<commit_message>
updated validation set for generation S1_A
</commit_message>
<xml_diff>
--- a/exploration/validation_dataset.xlsx
+++ b/exploration/validation_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\OneDrive - UT Cloud\Thesis\esg_extraction\exploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC82A27-6E9E-4868-9826-6D99F056C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630DF4D-4391-4B8D-8777-EEE05B8D283F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10605" yWindow="0" windowWidth="11078" windowHeight="12863" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S1_Retrieval" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="350">
   <si>
     <t>report_name</t>
   </si>
@@ -7679,138 +7679,6 @@
     <t>cs_reasoning</t>
   </si>
   <si>
-    <t>{'ANALYSIS': 'The disclosure provided by Continental in the annual report partially meets the requirements outlined for managing and disclosing material impacts, risks, and opportunities related to its own workforce. The company has detailed its processes for identifying and assessing impacts, risks, and opportunities, as well as the actions taken to address them. However, there is room for improvement in providing specific details on the types of employees impacted, the effectiveness of measures, and the tracking and assessment of these efforts.', 'SCORE': 75}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided in the annual report covers a wide range of aspects related to managing and disclosing material impacts, risks, and opportunities related to the company's own workforce. It includes discussions on policies, actions, and initiatives related to working conditions, mental health, training, and skills development. However, there is room for improvement in providing more specific details and metrics to fully meet all the outlined requirements.", 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The report's disclosure provided by the company addresses several key aspects related to managing and disclosing material impacts, risks, and opportunities related to its own workforce. The company discusses various topics such as health &amp; safety, employee rights, talent development, and diversity &amp; inclusion. However, the disclosure lacks specific details on certain aspects such as the processes for identifying and addressing negative impacts, tracking effectiveness of measures, and ensuring practices do not contribute to negative impacts. More quantitative data and specific examples would enhance the quality of disclosure.", 'SCORE': 75}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided in the annual report partially addresses the requirements for describing material risks and opportunities related to the company's impacts and dependencies on its own workforce. The report discusses various risks related to labor rights, workforce management, and skill development initiatives. However, it lacks specific details on actions planned to mitigate these risks and pursue opportunities, as well as the tracking and assessment of effectiveness. The report could benefit from more explicit information on these aspects to enhance transparency and accountability.", 'SCORE': 65}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided in the annual report adequately addresses the material risks and opportunities related to the company's impacts and dependencies on its own workforce. The report discusses various risks such as operational, legal, reputational, and social risks, along with opportunities related to employee engagement, skills development, and workforce diversity. It also outlines actions planned to mitigate risks and pursue opportunities. However, the report could enhance clarity by explicitly linking each risk and opportunity to specific groups within the workforce and providing more detailed information on the effectiveness tracking and assessment of mitigation actions.", 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided in the annual report partially addresses the ESRS recommendation point by discussing the material risks and opportunities related to the company's impacts and dependencies on its own workforce. While the report mentions actions taken and strategies in place, it lacks specific details on tracking and assessing the effectiveness of these actions. Additionally, there is a focus on workforce strategy and employee well-being, but limited information on opportunities related to the company's own workforce.", 'SCORE': 70}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The disclosure provided by Continental in their annual report regarding respect for human rights, including labor rights of their own workforce, is comprehensive and detailed. They address various aspects such as labor standards, policies alignment with international instruments, incidents of forced labor and child labor, penalties, and fines related to human rights violations. Continental also outlines their management approach, stakeholder engagement, and adherence to global standards. However, there is room for improvement in providing specific details on severe human rights incidents and reconciliation of fines, penalties, or compensation. Overall, the disclosure demonstrates a strong commitment to human rights.', 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a comprehensive overview of Schneider Electric's commitment to human rights, including labor rights, within its own workforce. The company aligns its sustainability strategy with the UN's principles, discloses its human rights policies, and addresses risks such as forced labor and mental health issues. Schneider Electric's detailed disclosure on its human rights due diligence process, living wage commitment, and partnerships demonstrates a strong focus on respecting human rights. However, the report could enhance disclosure by providing more specific details on identified severe human rights incidents and reconciliation efforts related to its own workforce.", 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided in the annual report demonstrates a strong commitment to human rights, including labor rights, within Philips' own workforce. The report covers various aspects such as policy commitments, human rights impact assessments, governance structures, grievance mechanisms, and engagement with stakeholders. Philips outlines its approach to respect for human rights and labor rights, aligning with international standards and conducting due diligence. However, the report lacks specific details on identified severe human rights incidents and the reconciliation of fines or penalties related to such incidents.", 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided in the annual report by Continental demonstrates a strong commitment to engaging with its own workers and workers' representatives. The company has addressed key aspects such as general approach to engagement, direct and indirect engagement with workers, assessment of effectiveness, steps to gain insight into vulnerable groups, and setting targets with workforce involvement. Continental's detailed descriptions and examples showcase a comprehensive engagement strategy.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided by Schneider Electric demonstrates a strong commitment to engaging with its workers and workers' representatives. The company discloses its approach to engagement, the stages and types of engagement, responsible roles, assessment of effectiveness, steps for vulnerable groups, and setting targets with workers. The disclosure also includes information on employee feedback mechanisms, action plans, and social dialogue policies. However, there is room for improvement in providing more specific details on the assessment of engagement effectiveness and steps taken for vulnerable groups.", 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided by the company partially meets the requirements for engaging with its workers and workers' representatives. The company discusses its engagement with employees, including regular meetings, surveys, and development processes. It also mentions collective bargaining agreements and social dialogue. However, the disclosure lacks specific details on how employee perspectives inform decision-making, steps taken to understand vulnerable groups, and direct engagement in setting targets. There is room for improvement in providing more comprehensive information.", 'SCORE': 75}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided by Continental AG in its annual report regarding preventing discrimination and advancing diversity and inclusion in its workforce is comprehensive and detailed. The company has addressed all the key requirements outlined, including specific policies, coverage of discrimination grounds, commitments to vulnerable groups, implementation procedures, and disclosure of incidents and fines. Continental AG's proactive approach to diversity and inclusion, setting targets, promoting internationality, gender diversity, and engaging with marginalized groups, demonstrates a strong commitment to fostering a diverse and inclusive workplace.", 'SCORE': 100}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided by Schneider Electric demonstrates a strong commitment to preventing discrimination and promoting diversity and inclusion in its workforce. The company has detailed policies and initiatives in place to address discrimination, harassment, and promote equal opportunities. Schneider Electric's approach to diversity and inclusion is comprehensive and well-documented throughout the report.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The company's annual report provides a comprehensive disclosure on its policies and practices related to preventing discrimination and promoting diversity and inclusion in its workforce. The report covers specific policies, grounds for discrimination, commitments to vulnerable groups, implementation procedures, disclosure of fines, and compensation. It also includes diversity metrics, employee resource groups, and external awards. However, there could be more detailed information on the implementation of policies and procedures to address discrimination once detected.", 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The disclosure provided by Continental in the annual report regarding processes to remediate negative impacts and channels for own workforce to raise concerns is comprehensive and detailed. The company has addressed several key requirements such as establishing dedicated mechanisms for employees to raise concerns, providing multiple channels for reporting, ensuring confidentiality and protection against retaliation, and implementing remediation processes. However, there are some areas where more specific details could be provided, such as explicit assessment of awareness and trust in the channels, and more transparency on the effectiveness of the integrity system.', 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided by Schneider Electric in their annual report demonstrates a comprehensive approach to addressing negative impacts in the workforce through various channels and policies. The company has detailed processes for remediation, clear channels for raising concerns, and mechanisms for protection against retaliation. Schneider Electric's commitment to fostering a speak-up culture and monitoring the effectiveness of their systems is evident throughout the disclosure.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The disclosure provided by the company regarding its approach to remediate negative impacts in the workforce is comprehensive and detailed. The company has outlined its SpeakUp program, reporting mechanisms, investigation processes, and follow-up actions taken. It discloses the number of concerns raised, types of concerns, regions of origin, substantiated cases, and actions taken. The company also emphasizes protection against retaliation and training for compliance officers. However, the disclosure lacks specific information on the general approach to providing remedy for negative impacts and the assessment of workforce awareness and trust in the reporting channels.', 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The disclosure provided in the annual report lacks specific information regarding the social protection coverage of the company's own workforce. While some general details about personnel expenses, employee benefits, and deferred compensation are mentioned, there is a notable absence of explicit information addressing the coverage of employees against major life events as outlined in the requirements. The report does not clearly indicate whether all employees are covered by social protection mechanisms or provide details on countries where employees lack such coverage.", 'SCORE': 30}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The disclosure provided by Schneider Electric regarding social protection for its workforce primarily focuses on family leave policies, well-being programs, and safety management systems. While the company emphasizes employee well-being and safety, it lacks specific details on social protection mechanisms against major life events like sickness, unemployment, and retirement. The report does not explicitly address whether all employees are covered by social protection or provide information on countries where employees lack such coverage.', 'SCORE': 60}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The disclosure provided by the company regarding social protection for its workforce is detailed and covers various aspects such as sickness, unemployment, employment injury, parental leave, and retirement. The report clearly outlines the countries where employees are not covered and the eligibility criteria in different regions. However, the report lacks specific details on the types of employees not covered in those countries, which is a key requirement for high-quality disclosure.', 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>cs LLM result</t>
-  </si>
-  <si>
-    <t>dd llm result</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The annual report provides a detailed and comprehensive disclosure on how the company manages and discloses material impacts, risks, and opportunities related to its own workforce. The report covers various aspects such as labor standards, adequate wages, work-life balance, training and skill development, secure employment, social dialogue, employee privacy, and occupational safety and health. The company has outlined specific processes, methodologies, and actions taken to address these areas, demonstrating a strong commitment to employee well-being and engagement.', 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The annual report provides a comprehensive overview of how Schneider Electric manages and discloses material impacts, risks, and opportunities related to its workforce. The report covers various aspects such as trust programs, whistleblowing policies, working conditions, mental health, double materiality assessment, sustainability matters, cybersecurity, employee engagement, training and skills development, and equal treatment. It includes detailed descriptions of policies, governance structures, initiatives, performance metrics, and recognition received. The company demonstrates a strong commitment to employee well-being, safety, diversity, and inclusion.', 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a detailed overview of how Philips manages and discloses material impacts, risks, and opportunities related to its own workforce. The report covers various aspects such as employee rights, health &amp; safety, talent development, diversity &amp; inclusion, and stakeholder engagement. It includes information on policies, metrics, targets, and the Double Materiality Assessment process. The report also highlights the company's commitment to transparency and engagement with stakeholders.", 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a detailed overview of the material risks and opportunities related to the company's impacts and dependencies on its own workforce. It covers various aspects such as training, skill development, secure employment, and potential risks like labor rights violations and workforce management challenges. The report also includes information on how these risks are managed and monitored. However, there is room for improvement in providing more specific quantitative data and targets related to these aspects.", 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a detailed and comprehensive disclosure on the material risks and opportunities related to the company's impacts and dependencies on its own workforce. It covers various aspects such as working conditions, employee health and safety, equal treatment and opportunities, training and skills development, and workforce diversity. The report also discusses the importance of talent acquisition, development, and retention, emphasizing critical skills and workforce diversity. Overall, the disclosure demonstrates a strong commitment to addressing workforce-related risks and opportunities.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a detailed overview of the company's approach to managing risks and opportunities related to its own workforce. It covers various aspects such as workforce strategy, employee rights, health &amp; safety, talent development, and human rights impacts. The report also addresses the challenges related to attracting and retaining talent. However, there is room for improvement in providing specific quantitative metrics and targets to enhance transparency and accountability.", 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a comprehensive overview of Continental's approach to respect for human rights, including labor rights, within its own workforce. The report covers various aspects such as management approaches, stakeholder engagement, due diligence processes, potential impacts, risks, and compliance with international frameworks. Continental's commitment to human rights and labor standards is well-documented, including specific policies, monitoring mechanisms, and adherence to global standards.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "Schneider Electric demonstrates a strong commitment to respecting human rights and labor rights within its own workforce. The company aligns its sustainability strategy with the UN's principles, actively participates in external initiatives, conducts thorough risk assessments, and implements robust policies and programs to address human rights issues. Schneider Electric's detailed disclosure on its approach to human rights, including efforts to prevent forced labor, ensure living wages, and support LGBT+ rights, showcases a comprehensive and proactive stance towards respecting human rights and labor rights.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a comprehensive overview of Philips' approach to respecting human rights, including labor rights, within its own workforce and value chain. The company demonstrates a strong commitment to identifying, preventing, and mitigating adverse human rights impacts. Philips conducts human rights due diligence, engages in human rights impact assessments, and has established governance and grievance mechanisms to uphold human rights standards. The report also highlights specific policies, metrics, and targets related to employee rights, fair employment, diversity &amp; inclusion, and collective bargaining. Overall, the disclosure is detailed, transparent, and aligned with international standards and best practices.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The company provides a detailed and comprehensive overview of its engagement with workers and workers' representatives. It outlines various channels and processes for communication, feedback, and involvement of employees in decision-making. The report highlights the integration of employee perspectives into strategic decisions and the consideration of their interests in various aspects of the business. The disclosure demonstrates a strong commitment to social dialogue and employee well-being.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a comprehensive overview of how Schneider Electric engages with its workers and workers' representatives. The company demonstrates a strong commitment to employee engagement through various initiatives, such as annual surveys, action plans, and social dialogue at both local and global levels. The report highlights the importance of two-way communication, feedback mechanisms, and the impact of employee engagement on business performance. Schneider Electric's approach to engaging with its workforce is well-documented and aligned with best practices in sustainability reporting.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a detailed overview of how Philips engages with its workers and workers' representatives. The company actively involves employees through various channels such as regular meetings, surveys, and engagement initiatives. Philips demonstrates a commitment to respecting employee rights, providing fair employment, and engaging in collective bargaining and social dialogue. The report also highlights specific initiatives related to employee engagement, talent development, and workplace culture. Overall, the disclosure is comprehensive and transparent, showcasing a strong focus on engaging with workers and workers' representatives.", 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The company provides a detailed and comprehensive disclosure regarding its efforts to prevent discrimination and advance diversity and inclusion in its workforce. It outlines specific targets, initiatives, processes, and monitoring mechanisms related to gender diversity and inclusion. The report also addresses potential risks and impacts related to discrimination and harassment, demonstrating a proactive approach to mitigating such issues.', 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a comprehensive overview of Schneider Electric's commitment to preventing discrimination and advancing diversity and inclusion in its workforce. The company outlines various initiatives, policies, and programs aimed at creating an inclusive environment, promoting diversity, and ensuring fair treatment for all employees. Schneider Electric's detailed disclosure demonstrates a strong focus on diversity, equity, and inclusion across various aspects of its operations.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The company provides a detailed and comprehensive disclosure regarding its commitment to preventing discrimination and advancing diversity and inclusion in its workforce. The report outlines specific policies, initiatives, metrics, and governance structures in place to promote a fair and inclusive workplace. It also includes information on diversity targets, employee resource groups, external awards, and monitoring mechanisms. The company's approach demonstrates a strong commitment to diversity and inclusion throughout the organization.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a detailed overview of Continental's processes and channels for remediating negative impacts and enabling its own workforce to raise concerns. The company has established comprehensive integrity mechanisms, including an integrity portal, hotline, and email, to address violations and protect whistleblowers. Various communication channels and training programs are in place to raise awareness and ensure effective implementation. Continental's approach to data protection and compliance with relevant regulations is well-documented. Overall, the report demonstrates a strong commitment to addressing workforce concerns and maintaining ethical standards.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a comprehensive overview of Schneider Electric's approaches to remediate negative impacts in the workforce through its Speak Up mindset, whistleblowing policies, committees for compliance and disciplinary actions, corrective measures, employee surveys, and protection mechanisms. The report details the governance structure, case management process, employee engagement initiatives, and commitment to human rights. The company's transparency in reporting and commitment to continuous improvement are evident throughout the disclosures.", 'SCORE': 95}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a detailed overview of the company's approach to remediate negative impacts in the workforce through its SpeakUp program, reporting mechanisms, investigation processes, and follow-up actions. It includes statistics on concerns raised, types of concerns, regional breakdowns, substantiated cases, remedial and disciplinary actions taken, and training initiatives. The report also highlights the protection of whistleblowers and the alignment with relevant legislation. However, there could be further details on specific case studies or examples of remedial actions taken to enhance transparency.", 'SCORE': 85}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a moderate level of disclosure regarding how the company protects its workforce through social protection. It mentions aspects such as labor standards, wages, social security contributions, pension provisions, and other benefits. However, the report lacks specific details on the company's social protection policies, initiatives, and the effectiveness of these measures in safeguarding employees' well-being.", 'SCORE': 65}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': "The annual report provides a comprehensive overview of Schneider Electric's efforts to protect its workforce through various initiatives such as the Global Family Leave Policy, Employee Assistance Program, back-up family care benefits, and access to healthcare. The report also includes details on social protection, health and safety management systems, and pension benefits. Schneider Electric's commitment to social protection and well-being is evident through its alignment with global standards and recognition of diverse workforce needs.", 'SCORE': 90}</t>
-  </si>
-  <si>
-    <t>{'ANALYSIS': 'The annual report provides a detailed overview of the social protection measures provided to employees in various countries, including coverage for sickness, unemployment, employment injury, parental leave, and retirement. The report specifies eligibility criteria and variations in benefits based on local regulations and practices. However, there could be further enhancement by providing more specific data on the percentage of employees covered in each category and the overall effectiveness of these social protection programs.', 'SCORE': 85}</t>
-  </si>
-  <si>
     <t>(+) coverage of different dimensions of social protection (sickness, unemployment, parental leave, …) and region specific details
 (-) company identifies where government coverage is non-existent or insufficient and clarifies whether Philips supplements it or not
 (-) no monitoring, governance mechanisms disclosed</t>
@@ -7893,11 +7761,6 @@
   </si>
   <si>
     <t>(-) only shortcoming: lack  of disclosure of actual grievances or remediation outcomes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes: 
-How reliable is the information?
-</t>
   </si>
   <si>
     <t>(+) high detail of engagement methods and platforms
@@ -7986,6 +7849,24 @@
   <si>
     <t>(-) does not provide a clear picture of the financial and human resources allocated to manage  material impacts
 (-) room for improvement in providing specific details on the types of employees impacted, the effectiveness of measures, and the tracking and assessment of these efforts</t>
+  </si>
+  <si>
+    <t>(+) broad and detailed set of policies, actions, and governance structures, including metrics, survey data, and qualitative insights
+(+) Initiatives and programs are well-described and contextualized
+(-) some granularity is lacking, particularly with respect to vulnerable subgroups</t>
+  </si>
+  <si>
+    <t>(-) no mention of at-risk characteristics or contexts of vulnerable groups
+(-) weak disclosure of transition-related impacts</t>
+  </si>
+  <si>
+    <t>(+) detailes overview with clear examples (program plans and governance structures)
+(+) compliance with international instruments
+(-) lack of specific breakdowns of impacts by employee types in some areas</t>
+  </si>
+  <si>
+    <t>(-) limited information on impact of transition plans and vulnerable groups 
+(-) risk identification processes are broadly described, specific methodologies per risk area (e.g., health &amp; safety vs. human rights) could be more detailed</t>
   </si>
 </sst>
 </file>
@@ -8015,18 +7896,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -8070,21 +7945,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -8369,8 +8244,8 @@
   <dimension ref="A1:D283"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29:C219"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C190" sqref="C190:C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11496,7 +11371,7 @@
       <c r="B223" t="s">
         <v>35</v>
       </c>
-      <c r="C223" s="5" t="s">
+      <c r="C223" s="4" t="s">
         <v>238</v>
       </c>
       <c r="D223" s="3" t="s">
@@ -12367,78 +12242,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF936B0-06A1-4D6F-B394-60C114961257}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.19921875" customWidth="1"/>
-    <col min="2" max="2" width="4.59765625" customWidth="1"/>
-    <col min="3" max="3" width="6.19921875" customWidth="1"/>
-    <col min="4" max="4" width="34.86328125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="7.06640625" customWidth="1"/>
-    <col min="7" max="7" width="27.86328125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="46.19921875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.796875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="8.06640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.86328125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="40.265625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="6" width="39.265625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="10.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>90</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="E2" s="6">
         <v>70</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F2" s="7" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -12449,22 +12311,16 @@
         <v>85</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="F3" s="6">
+        <v>342</v>
+      </c>
+      <c r="E3" s="6">
         <v>75</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F3" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -12475,22 +12331,16 @@
         <v>95</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="F4" s="6">
+        <v>332</v>
+      </c>
+      <c r="E4" s="6">
         <v>90</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F4" s="7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -12501,22 +12351,16 @@
         <v>80</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>375</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="F5" s="6">
+        <v>330</v>
+      </c>
+      <c r="E5" s="6">
         <v>90</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="6" customFormat="1" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F5" s="7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="23.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -12527,22 +12371,16 @@
         <v>95</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="F6" s="6">
+        <v>320</v>
+      </c>
+      <c r="E6" s="6">
         <v>100</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F6" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -12553,22 +12391,16 @@
         <v>80</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="F7" s="6">
+        <v>317</v>
+      </c>
+      <c r="E7" s="6">
         <v>65</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F7" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
@@ -12579,88 +12411,76 @@
         <v>65</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="F8" s="8">
+        <v>312</v>
+      </c>
+      <c r="E8" s="8">
         <v>30</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>363</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="228" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="F8" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="6" customFormat="1" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C9" s="10">
+        <v>95</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="E9" s="10">
+        <v>85</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>85</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="F10" s="10">
+        <v>340</v>
+      </c>
+      <c r="E10" s="6">
         <v>80</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F10" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>120</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="6">
         <v>80</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="F11" s="10">
+        <v>334</v>
+      </c>
+      <c r="E11" s="6">
         <v>75</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F11" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>120</v>
       </c>
@@ -12671,22 +12491,16 @@
         <v>95</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="F12" s="6">
+        <v>328</v>
+      </c>
+      <c r="E12" s="6">
         <v>90</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F12" s="7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>120</v>
       </c>
@@ -12697,22 +12511,16 @@
         <v>90</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="F13" s="6">
+        <v>322</v>
+      </c>
+      <c r="E13" s="6">
         <v>90</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F13" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>120</v>
       </c>
@@ -12723,22 +12531,16 @@
         <v>95</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="F14" s="6">
+        <v>315</v>
+      </c>
+      <c r="E14" s="6">
         <v>95</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="8" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F14" s="7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>120</v>
       </c>
@@ -12749,88 +12551,76 @@
         <v>80</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="F15" s="8">
+        <v>311</v>
+      </c>
+      <c r="E15" s="8">
         <v>60</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="F15" s="9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="10">
+        <v>90</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E16" s="10">
+        <v>85</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="24.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>237</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="6">
         <v>80</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>384</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="F17" s="10">
+        <v>339</v>
+      </c>
+      <c r="E17" s="6">
         <v>70</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F17" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>237</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="6">
         <v>95</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="F18" s="10">
+        <v>336</v>
+      </c>
+      <c r="E18" s="6">
         <v>85</v>
       </c>
-      <c r="G18" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="30.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F18" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30.85" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>237</v>
       </c>
@@ -12841,22 +12631,16 @@
         <v>90</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="F19" s="6">
+        <v>326</v>
+      </c>
+      <c r="E19" s="6">
         <v>85</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F19" s="7" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>237</v>
       </c>
@@ -12867,22 +12651,16 @@
         <v>90</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="F20" s="6">
+        <v>324</v>
+      </c>
+      <c r="E20" s="6">
         <v>90</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F20" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>237</v>
       </c>
@@ -12893,22 +12671,16 @@
         <v>90</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="F21" s="6">
+        <v>313</v>
+      </c>
+      <c r="E21" s="6">
         <v>90</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F21" s="7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>237</v>
       </c>
@@ -12919,24 +12691,13 @@
         <v>90</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="F22" s="6">
+        <v>308</v>
+      </c>
+      <c r="E22" s="6">
         <v>100</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="D26" s="5" t="s">
-        <v>370</v>
+      <c r="F22" s="7" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>